<commit_message>
code and data commit
code and data are all completed apart from cleaning. report gained some words.
</commit_message>
<xml_diff>
--- a/Excel/Tables of results.xlsx
+++ b/Excel/Tables of results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Uni\FINAL_Year\Dissertation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4645539-B746-4B01-94B3-FEF2195ED9F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA9118C-43AB-438F-ACF2-DFBDF30F8AFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A522EAAA-04A2-4FA9-A435-DE8F63DB9FA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A522EAAA-04A2-4FA9-A435-DE8F63DB9FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="52">
   <si>
     <t>filter 1</t>
   </si>
@@ -172,6 +173,24 @@
   <si>
     <t>Original file 5</t>
   </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>track 1 + vaccum</t>
+  </si>
+  <si>
+    <t>track 2 + vaccum</t>
+  </si>
+  <si>
+    <t>track 3 + vaccum</t>
+  </si>
+  <si>
+    <t>track 4 + vaccum</t>
+  </si>
+  <si>
+    <t>track 5 + vaccum</t>
+  </si>
 </sst>
 </file>
 
@@ -224,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -251,6 +270,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1069,7 +1098,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.7306757794139339E-2"/>
+          <c:y val="0.21111876904799418"/>
+          <c:w val="0.95212234098070758"/>
+          <c:h val="0.7338778348579662"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1103,29 +1142,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$W$55:$Z$55</c:f>
+              <c:f>Sheet1!$W$55:$Y$55</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>correlation to file</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>correlation to recorded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$56:$Z$56</c:f>
+              <c:f>Sheet1!$W$56:$Y$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>9.5328478222646146E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.4608788668361524E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1165,29 +1210,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$W$55:$Z$55</c:f>
+              <c:f>Sheet1!$W$55:$Y$55</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>correlation to file</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>correlation to recorded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$57:$Z$57</c:f>
+              <c:f>Sheet1!$W$57:$Y$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.23016581808913311</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9323681228287359E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5971460000000013E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1227,29 +1278,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$W$55:$Z$55</c:f>
+              <c:f>Sheet1!$W$55:$Y$55</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>correlation to file</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>correlation to recorded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$58:$Z$58</c:f>
+              <c:f>Sheet1!$W$58:$Y$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.22984919364443918</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.2811126700233316E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9133000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1289,29 +1346,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$W$55:$Z$55</c:f>
+              <c:f>Sheet1!$W$55:$Y$55</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>correlation to file</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>correlation to recorded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$59:$Z$59</c:f>
+              <c:f>Sheet1!$W$59:$Y$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.12602352499530695</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.4245149648056203E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.2414722999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1351,29 +1414,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$W$55:$Z$55</c:f>
+              <c:f>Sheet1!$W$55:$Y$55</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>correlation to file</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>correlation to recorded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$60:$Z$60</c:f>
+              <c:f>Sheet1!$W$60:$Y$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.23775255678971363</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.10386996855845942</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4373999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1413,29 +1482,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$W$55:$Z$55</c:f>
+              <c:f>Sheet1!$W$55:$Y$55</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>correlation to file</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>correlation to recorded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$61:$Z$61</c:f>
+              <c:f>Sheet1!$W$61:$Y$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3.4631245452790463E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.2445791483400096E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3941437399999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3100,10 +3175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A489FFF-CD10-4825-B7D5-0A9170441D4E}">
-  <dimension ref="F4:AA61"/>
+  <dimension ref="F4:AA78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3138,6 +3213,7 @@
       <c r="V4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Y4" s="10"/>
     </row>
     <row r="5" spans="6:27" x14ac:dyDescent="0.25">
       <c r="G5" s="1" t="s">
@@ -3169,6 +3245,9 @@
       </c>
       <c r="X5" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="6:27" x14ac:dyDescent="0.25">
@@ -3211,6 +3290,9 @@
       <c r="X6" s="2">
         <v>-9.6599427807263899E-4</v>
       </c>
+      <c r="Y6" s="12">
+        <v>0</v>
+      </c>
       <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="6:27" x14ac:dyDescent="0.25">
@@ -3232,7 +3314,7 @@
       <c r="K7" s="1">
         <v>-3.2697765766460398E-4</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -3249,7 +3331,7 @@
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="14" t="s">
         <v>4</v>
       </c>
       <c r="V7" s="1" t="s">
@@ -3260,6 +3342,9 @@
       </c>
       <c r="X7" s="2">
         <v>3.2023509679633402E-3</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>7.6504100000000005E-2</v>
       </c>
       <c r="AA7" s="2"/>
     </row>
@@ -3282,7 +3367,7 @@
       <c r="K8" s="1">
         <v>7.7372479303842801E-3</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="1" t="s">
         <v>31</v>
       </c>
@@ -3297,7 +3382,7 @@
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-      <c r="U8" s="10"/>
+      <c r="U8" s="14"/>
       <c r="V8" s="1" t="s">
         <v>1</v>
       </c>
@@ -3306,6 +3391,9 @@
       </c>
       <c r="X8" s="2">
         <v>4.4309307214132204E-3</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>5.8640699999999997E-2</v>
       </c>
       <c r="AA8" s="2"/>
     </row>
@@ -3328,7 +3416,7 @@
       <c r="K9" s="1">
         <v>-3.1102899338873902E-3</v>
       </c>
-      <c r="M9" s="10"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
@@ -3343,7 +3431,7 @@
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-      <c r="U9" s="10" t="s">
+      <c r="U9" s="14" t="s">
         <v>5</v>
       </c>
       <c r="V9" s="1" t="s">
@@ -3354,6 +3442,9 @@
       </c>
       <c r="X9" s="2">
         <v>-8.9328675066072602E-3</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>7.242197</v>
       </c>
       <c r="AA9" s="2"/>
     </row>
@@ -3376,7 +3467,7 @@
       <c r="K10" s="1">
         <v>1</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -3393,7 +3484,7 @@
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="U10" s="10"/>
+      <c r="U10" s="14"/>
       <c r="V10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3402,6 +3493,9 @@
       </c>
       <c r="X10" s="2">
         <v>5.8828764724569802E-3</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>5.1037199999999998E-2</v>
       </c>
       <c r="AA10" s="2"/>
     </row>
@@ -3410,7 +3504,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="M11" s="10"/>
+      <c r="M11" s="14"/>
       <c r="N11" s="2" t="s">
         <v>33</v>
       </c>
@@ -3430,6 +3524,9 @@
       </c>
       <c r="X11" s="2">
         <v>-6.0976098356833701E-3</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>2.3985560000000001</v>
       </c>
       <c r="AA11" s="2"/>
     </row>
@@ -3442,6 +3539,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="Q12" s="5"/>
+      <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="6:27" x14ac:dyDescent="0.25">
       <c r="G13" s="1" t="s">
@@ -3460,6 +3558,7 @@
         <v>45</v>
       </c>
       <c r="Q13" s="5"/>
+      <c r="Y13" s="12"/>
     </row>
     <row r="14" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F14" s="1" t="s">
@@ -3487,6 +3586,7 @@
       </c>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
+      <c r="Y14" s="11"/>
     </row>
     <row r="15" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F15" s="2" t="s">
@@ -3527,6 +3627,9 @@
       <c r="X15" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="Y15" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="6:27" x14ac:dyDescent="0.25">
@@ -3571,6 +3674,9 @@
       <c r="X16" s="6">
         <v>-8.7681676216278302E-5</v>
       </c>
+      <c r="Y16" s="11">
+        <v>0</v>
+      </c>
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="6:27" x14ac:dyDescent="0.25">
@@ -3587,7 +3693,7 @@
       <c r="J17" s="3">
         <v>-0.139950017882363</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="M17" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N17" s="2" t="s">
@@ -3605,7 +3711,7 @@
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
-      <c r="U17" s="10" t="s">
+      <c r="U17" s="14" t="s">
         <v>4</v>
       </c>
       <c r="V17" s="2" t="s">
@@ -3616,6 +3722,9 @@
       </c>
       <c r="X17" s="2">
         <v>2.26964265601475E-3</v>
+      </c>
+      <c r="Y17" s="11">
+        <v>7.2289999999999993E-2</v>
       </c>
       <c r="AA17" s="2"/>
     </row>
@@ -3638,7 +3747,7 @@
       <c r="K18" s="1">
         <v>0.42807982748315199</v>
       </c>
-      <c r="M18" s="10"/>
+      <c r="M18" s="14"/>
       <c r="N18" s="2" t="s">
         <v>31</v>
       </c>
@@ -3654,7 +3763,7 @@
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
-      <c r="U18" s="10"/>
+      <c r="U18" s="14"/>
       <c r="V18" s="2" t="s">
         <v>31</v>
       </c>
@@ -3663,6 +3772,9 @@
       </c>
       <c r="X18" s="2">
         <v>3.65437069348789E-4</v>
+      </c>
+      <c r="Y18" s="11">
+        <v>6.4107200000000003E-2</v>
       </c>
       <c r="AA18" s="2"/>
     </row>
@@ -3671,7 +3783,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="M19" s="10"/>
+      <c r="M19" s="14"/>
       <c r="N19" s="2" t="s">
         <v>34</v>
       </c>
@@ -3687,7 +3799,7 @@
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
-      <c r="U19" s="10"/>
+      <c r="U19" s="14"/>
       <c r="V19" s="2" t="s">
         <v>34</v>
       </c>
@@ -3696,6 +3808,9 @@
       </c>
       <c r="X19" s="2">
         <v>-1.65960943944583E-3</v>
+      </c>
+      <c r="Y19" s="11">
+        <v>7.2935926999999996</v>
       </c>
       <c r="AA19" s="2"/>
     </row>
@@ -3707,7 +3822,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="14" t="s">
         <v>5</v>
       </c>
       <c r="N20" s="2" t="s">
@@ -3725,7 +3840,7 @@
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
-      <c r="U20" s="10" t="s">
+      <c r="U20" s="14" t="s">
         <v>5</v>
       </c>
       <c r="V20" s="2" t="s">
@@ -3736,6 +3851,9 @@
       </c>
       <c r="X20" s="2">
         <v>-4.01291877554331E-3</v>
+      </c>
+      <c r="Y20" s="11">
+        <v>5.4161800000000003E-2</v>
       </c>
       <c r="AA20" s="2"/>
     </row>
@@ -3755,7 +3873,7 @@
       <c r="K21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="10"/>
+      <c r="M21" s="14"/>
       <c r="N21" s="2" t="s">
         <v>33</v>
       </c>
@@ -3771,7 +3889,7 @@
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
-      <c r="U21" s="10"/>
+      <c r="U21" s="14"/>
       <c r="V21" s="2" t="s">
         <v>33</v>
       </c>
@@ -3780,6 +3898,9 @@
       </c>
       <c r="X21" s="2">
         <v>3.69627838604504E-3</v>
+      </c>
+      <c r="Y21" s="11">
+        <v>2.3575537</v>
       </c>
       <c r="AA21" s="2"/>
     </row>
@@ -3811,6 +3932,7 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
+      <c r="Y22" s="11"/>
     </row>
     <row r="23" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F23" s="1" t="s">
@@ -3840,6 +3962,7 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
+      <c r="Y23" s="11"/>
     </row>
     <row r="24" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F24" s="1" t="s">
@@ -3874,6 +3997,7 @@
       </c>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
+      <c r="Y24" s="11"/>
     </row>
     <row r="25" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F25" s="1" t="s">
@@ -3914,6 +4038,9 @@
       <c r="X25" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="Y25" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="6:27" x14ac:dyDescent="0.25">
@@ -3961,10 +4088,13 @@
       <c r="X26" s="2">
         <v>4.6717623414625401E-4</v>
       </c>
+      <c r="Y26" s="11">
+        <v>0</v>
+      </c>
       <c r="AA26" s="2"/>
     </row>
     <row r="27" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="M27" s="10" t="s">
+      <c r="M27" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N27" s="2" t="s">
@@ -3982,7 +4112,7 @@
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
-      <c r="U27" s="10" t="s">
+      <c r="U27" s="14" t="s">
         <v>4</v>
       </c>
       <c r="V27" s="2" t="s">
@@ -3994,10 +4124,13 @@
       <c r="X27" s="2">
         <v>5.9846528988085198E-3</v>
       </c>
+      <c r="Y27" s="11">
+        <v>0.12706500000000001</v>
+      </c>
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="M28" s="10"/>
+      <c r="M28" s="14"/>
       <c r="N28" s="2" t="s">
         <v>31</v>
       </c>
@@ -4013,7 +4146,7 @@
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
-      <c r="U28" s="10"/>
+      <c r="U28" s="14"/>
       <c r="V28" s="2" t="s">
         <v>31</v>
       </c>
@@ -4023,10 +4156,13 @@
       <c r="X28" s="2">
         <v>5.57485038279749E-3</v>
       </c>
+      <c r="Y28" s="11">
+        <v>5.5505600000000002E-2</v>
+      </c>
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="M29" s="10"/>
+      <c r="M29" s="14"/>
       <c r="N29" s="2" t="s">
         <v>34</v>
       </c>
@@ -4042,7 +4178,7 @@
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
-      <c r="U29" s="10"/>
+      <c r="U29" s="14"/>
       <c r="V29" s="2" t="s">
         <v>34</v>
       </c>
@@ -4052,10 +4188,13 @@
       <c r="X29" s="2">
         <v>-1.6121990973710702E-2</v>
       </c>
+      <c r="Y29" s="11">
+        <v>7.2236172999999999</v>
+      </c>
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="M30" s="10" t="s">
+      <c r="M30" s="14" t="s">
         <v>5</v>
       </c>
       <c r="N30" s="2" t="s">
@@ -4073,7 +4212,7 @@
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
-      <c r="U30" s="10" t="s">
+      <c r="U30" s="14" t="s">
         <v>5</v>
       </c>
       <c r="V30" s="2" t="s">
@@ -4084,6 +4223,9 @@
       </c>
       <c r="X30" s="2">
         <v>8.9263890964573194E-3</v>
+      </c>
+      <c r="Y30" s="11">
+        <v>5.3828899999999999E-2</v>
       </c>
       <c r="AA30" s="2"/>
     </row>
@@ -4096,7 +4238,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
-      <c r="M31" s="10"/>
+      <c r="M31" s="14"/>
       <c r="N31" s="2" t="s">
         <v>33</v>
       </c>
@@ -4112,13 +4254,16 @@
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
-      <c r="U31" s="10"/>
+      <c r="U31" s="14"/>
       <c r="V31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="W31" s="2"/>
       <c r="X31" s="2">
         <v>-1.4261242992881701E-2</v>
+      </c>
+      <c r="Y31" s="11">
+        <v>2.3696328000000002</v>
       </c>
       <c r="AA31" s="2"/>
     </row>
@@ -4148,6 +4293,7 @@
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
+      <c r="Y32" s="11"/>
     </row>
     <row r="33" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F33" s="2" t="s">
@@ -4173,6 +4319,7 @@
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
+      <c r="Y33" s="11"/>
     </row>
     <row r="34" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F34" s="2" t="s">
@@ -4212,6 +4359,7 @@
       </c>
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
+      <c r="Y34" s="11"/>
     </row>
     <row r="35" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F35" s="2" t="s">
@@ -4254,6 +4402,9 @@
       <c r="X35" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="Y35" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="6:27" x14ac:dyDescent="0.25">
@@ -4300,6 +4451,9 @@
       <c r="X36" s="2">
         <v>1.6242434466186399E-3</v>
       </c>
+      <c r="Y36" s="11">
+        <v>0</v>
+      </c>
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="6:27" x14ac:dyDescent="0.25">
@@ -4326,7 +4480,7 @@
         <f t="shared" si="1"/>
         <v>0.42807982748315199</v>
       </c>
-      <c r="M37" s="10" t="s">
+      <c r="M37" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N37" s="2" t="s">
@@ -4344,7 +4498,7 @@
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
-      <c r="U37" s="10" t="s">
+      <c r="U37" s="14" t="s">
         <v>4</v>
       </c>
       <c r="V37" s="2" t="s">
@@ -4355,13 +4509,16 @@
       </c>
       <c r="X37" s="2">
         <v>-7.1643521232501598E-3</v>
+      </c>
+      <c r="Y37" s="11">
+        <v>7.6222399999999996E-2</v>
       </c>
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="6:27" x14ac:dyDescent="0.25">
       <c r="G38" s="3"/>
       <c r="H38" s="2"/>
-      <c r="M38" s="10"/>
+      <c r="M38" s="14"/>
       <c r="N38" s="2" t="s">
         <v>31</v>
       </c>
@@ -4377,7 +4534,7 @@
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
-      <c r="U38" s="10"/>
+      <c r="U38" s="14"/>
       <c r="V38" s="2" t="s">
         <v>31</v>
       </c>
@@ -4386,13 +4543,16 @@
       </c>
       <c r="X38" s="2">
         <v>-7.6358743501450301E-3</v>
+      </c>
+      <c r="Y38" s="11">
+        <v>5.5583500000000001E-2</v>
       </c>
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="6:27" x14ac:dyDescent="0.25">
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="M39" s="10"/>
+      <c r="M39" s="14"/>
       <c r="N39" s="2" t="s">
         <v>34</v>
       </c>
@@ -4408,7 +4568,7 @@
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
-      <c r="U39" s="10"/>
+      <c r="U39" s="14"/>
       <c r="V39" s="2" t="s">
         <v>34</v>
       </c>
@@ -4417,13 +4577,16 @@
       </c>
       <c r="X39" s="2">
         <v>2.9336220802583099E-3</v>
+      </c>
+      <c r="Y39" s="11">
+        <v>7.2306261999999997</v>
       </c>
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="6:27" x14ac:dyDescent="0.25">
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="M40" s="10" t="s">
+      <c r="M40" s="14" t="s">
         <v>5</v>
       </c>
       <c r="N40" s="2" t="s">
@@ -4441,7 +4604,7 @@
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
-      <c r="U40" s="10" t="s">
+      <c r="U40" s="14" t="s">
         <v>5</v>
       </c>
       <c r="V40" s="2" t="s">
@@ -4452,13 +4615,16 @@
       </c>
       <c r="X40" s="2">
         <v>-6.75607990422856E-3</v>
+      </c>
+      <c r="Y40" s="11">
+        <v>5.9511700000000001E-2</v>
       </c>
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="6:27" x14ac:dyDescent="0.25">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="M41" s="10"/>
+      <c r="M41" s="14"/>
       <c r="N41" s="2" t="s">
         <v>33</v>
       </c>
@@ -4474,7 +4640,7 @@
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
-      <c r="U41" s="10"/>
+      <c r="U41" s="14"/>
       <c r="V41" s="2" t="s">
         <v>33</v>
       </c>
@@ -4483,6 +4649,9 @@
       </c>
       <c r="X41" s="2">
         <v>5.4067183648593602E-3</v>
+      </c>
+      <c r="Y41" s="11">
+        <v>2.3848004999999999</v>
       </c>
       <c r="AA41" s="2"/>
     </row>
@@ -4496,6 +4665,7 @@
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
+      <c r="Y42" s="11"/>
     </row>
     <row r="43" spans="6:27" x14ac:dyDescent="0.25">
       <c r="P43" s="2"/>
@@ -4507,6 +4677,7 @@
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
+      <c r="Y43" s="11"/>
     </row>
     <row r="44" spans="6:27" x14ac:dyDescent="0.25">
       <c r="N44" s="1" t="s">
@@ -4523,6 +4694,7 @@
       </c>
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
+      <c r="Y44" s="11"/>
     </row>
     <row r="45" spans="6:27" x14ac:dyDescent="0.25">
       <c r="O45" s="2" t="s">
@@ -4545,6 +4717,9 @@
       <c r="X45" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="Y45" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="6:27" x14ac:dyDescent="0.25">
@@ -4574,10 +4749,13 @@
       <c r="X46" s="2">
         <v>9.1592986991269505E-3</v>
       </c>
+      <c r="Y46" s="11">
+        <v>0</v>
+      </c>
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="M47" s="10" t="s">
+      <c r="M47" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N47" s="2" t="s">
@@ -4595,7 +4773,7 @@
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
-      <c r="U47" s="10" t="s">
+      <c r="U47" s="14" t="s">
         <v>4</v>
       </c>
       <c r="V47" s="2" t="s">
@@ -4607,10 +4785,13 @@
       <c r="X47" s="2">
         <v>0.12799740749540001</v>
       </c>
+      <c r="Y47" s="11">
+        <v>7.7775800000000006E-2</v>
+      </c>
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="M48" s="10"/>
+      <c r="M48" s="14"/>
       <c r="N48" s="2" t="s">
         <v>31</v>
       </c>
@@ -4626,7 +4807,7 @@
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
-      <c r="U48" s="10"/>
+      <c r="U48" s="14"/>
       <c r="V48" s="2" t="s">
         <v>31</v>
       </c>
@@ -4636,10 +4817,13 @@
       <c r="X48" s="2">
         <v>0.24604854097746201</v>
       </c>
+      <c r="Y48" s="11">
+        <v>6.1828000000000001E-2</v>
+      </c>
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M49" s="10"/>
+      <c r="M49" s="14"/>
       <c r="N49" s="2" t="s">
         <v>34</v>
       </c>
@@ -4655,7 +4839,7 @@
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
-      <c r="U49" s="10"/>
+      <c r="U49" s="14"/>
       <c r="V49" s="2" t="s">
         <v>34</v>
       </c>
@@ -4665,10 +4849,13 @@
       <c r="X49" s="2">
         <v>-9.1577658240258902E-2</v>
       </c>
+      <c r="Y49" s="11">
+        <v>7.2173283000000001</v>
+      </c>
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M50" s="10" t="s">
+      <c r="M50" s="14" t="s">
         <v>5</v>
       </c>
       <c r="N50" s="2" t="s">
@@ -4686,7 +4873,7 @@
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
-      <c r="U50" s="10" t="s">
+      <c r="U50" s="14" t="s">
         <v>5</v>
       </c>
       <c r="V50" s="2" t="s">
@@ -4698,10 +4885,13 @@
       <c r="X50" s="2">
         <v>0.49377157854361098</v>
       </c>
+      <c r="Y50" s="11">
+        <v>5.33304E-2</v>
+      </c>
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M51" s="10"/>
+      <c r="M51" s="14"/>
       <c r="N51" s="2" t="s">
         <v>33</v>
       </c>
@@ -4717,7 +4907,7 @@
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
-      <c r="U51" s="10"/>
+      <c r="U51" s="14"/>
       <c r="V51" s="2" t="s">
         <v>33</v>
       </c>
@@ -4726,6 +4916,9 @@
       </c>
       <c r="X51" s="2">
         <v>-0.23276710783753099</v>
+      </c>
+      <c r="Y51" s="11">
+        <v>2.4601757000000002</v>
       </c>
       <c r="AA51" s="2"/>
     </row>
@@ -4739,6 +4932,7 @@
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
+      <c r="Y52" s="11"/>
     </row>
     <row r="53" spans="13:27" x14ac:dyDescent="0.25">
       <c r="P53" s="2"/>
@@ -4750,6 +4944,7 @@
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>
       <c r="X53" s="2"/>
+      <c r="Y53" s="11"/>
     </row>
     <row r="54" spans="13:27" x14ac:dyDescent="0.25">
       <c r="P54" s="2"/>
@@ -4761,6 +4956,7 @@
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
+      <c r="Y54" s="11"/>
     </row>
     <row r="55" spans="13:27" x14ac:dyDescent="0.25">
       <c r="O55" s="2" t="s">
@@ -4783,6 +4979,9 @@
       <c r="X55" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="Y55" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="56" spans="13:27" x14ac:dyDescent="0.25">
       <c r="M56" s="2" t="s">
@@ -4796,7 +4995,7 @@
         <v>3.5742566400714425E-3</v>
       </c>
       <c r="P56" s="2">
-        <f t="shared" ref="P56:R56" si="2">AVERAGE(ABS(P6),ABS(P16),ABS(P26),ABS(P36),ABS(P46))</f>
+        <f t="shared" ref="P56:Q56" si="2">AVERAGE(ABS(P6),ABS(P16),ABS(P26),ABS(P36),ABS(P46))</f>
         <v>1.5078519461113091E-2</v>
       </c>
       <c r="Q56" s="2">
@@ -4813,24 +5012,27 @@
         <v>12</v>
       </c>
       <c r="W56" s="2">
-        <f t="shared" ref="W56:Z56" si="3">AVERAGE(ABS(W6),ABS(W16),ABS(W26),ABS(W36),ABS(W46))</f>
+        <f t="shared" ref="W56:X56" si="3">AVERAGE(ABS(W6),ABS(W16),ABS(W26),ABS(W36),ABS(W46))</f>
         <v>9.5328478222646146E-3</v>
       </c>
       <c r="X56" s="2">
         <f t="shared" si="3"/>
         <v>2.4608788668361524E-3</v>
       </c>
+      <c r="Y56" s="11">
+        <v>0</v>
+      </c>
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M57" s="10" t="s">
+      <c r="M57" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>30</v>
       </c>
       <c r="O57" s="2">
-        <f t="shared" ref="O57:R61" si="4">AVERAGE(ABS(O7),ABS(O17),ABS(O27),ABS(O37),ABS(O47))</f>
+        <f t="shared" ref="O57:Q61" si="4">AVERAGE(ABS(O7),ABS(O17),ABS(O27),ABS(O37),ABS(O47))</f>
         <v>0.2217793285054365</v>
       </c>
       <c r="P57" s="2">
@@ -4844,24 +5046,27 @@
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
-      <c r="U57" s="10" t="s">
+      <c r="U57" s="14" t="s">
         <v>4</v>
       </c>
       <c r="V57" s="2" t="s">
         <v>30</v>
       </c>
       <c r="W57" s="2">
-        <f t="shared" ref="W57:Z57" si="5">AVERAGE(ABS(W7),ABS(W17),ABS(W27),ABS(W37),ABS(W47))</f>
+        <f t="shared" ref="W57:X57" si="5">AVERAGE(ABS(W7),ABS(W17),ABS(W27),ABS(W37),ABS(W47))</f>
         <v>0.23016581808913311</v>
       </c>
       <c r="X57" s="2">
         <f t="shared" si="5"/>
         <v>2.9323681228287359E-2</v>
       </c>
+      <c r="Y57" s="11">
+        <v>8.5971460000000013E-2</v>
+      </c>
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M58" s="10"/>
+      <c r="M58" s="14"/>
       <c r="N58" s="2" t="s">
         <v>31</v>
       </c>
@@ -4880,22 +5085,25 @@
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
-      <c r="U58" s="10"/>
+      <c r="U58" s="14"/>
       <c r="V58" s="2" t="s">
         <v>31</v>
       </c>
       <c r="W58" s="2">
-        <f t="shared" ref="W58:Z58" si="6">AVERAGE(ABS(W8),ABS(W18),ABS(W28),ABS(W38),ABS(W48))</f>
+        <f t="shared" ref="W58:X58" si="6">AVERAGE(ABS(W8),ABS(W18),ABS(W28),ABS(W38),ABS(W48))</f>
         <v>0.22984919364443918</v>
       </c>
       <c r="X58" s="2">
         <f t="shared" si="6"/>
         <v>5.2811126700233316E-2</v>
       </c>
+      <c r="Y58" s="11">
+        <v>5.9133000000000005E-2</v>
+      </c>
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M59" s="10"/>
+      <c r="M59" s="14"/>
       <c r="N59" s="2" t="s">
         <v>34</v>
       </c>
@@ -4914,22 +5122,25 @@
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
-      <c r="U59" s="10"/>
+      <c r="U59" s="14"/>
       <c r="V59" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W59" s="2">
-        <f t="shared" ref="W59:Z59" si="7">AVERAGE(ABS(W9),ABS(W19),ABS(W29),ABS(W39),ABS(W49))</f>
+        <f t="shared" ref="W59:X59" si="7">AVERAGE(ABS(W9),ABS(W19),ABS(W29),ABS(W39),ABS(W49))</f>
         <v>0.12602352499530695</v>
       </c>
       <c r="X59" s="2">
         <f t="shared" si="7"/>
         <v>2.4245149648056203E-2</v>
       </c>
+      <c r="Y59" s="11">
+        <v>7.2414722999999999</v>
+      </c>
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M60" s="10" t="s">
+      <c r="M60" s="14" t="s">
         <v>5</v>
       </c>
       <c r="N60" s="2" t="s">
@@ -4950,24 +5161,27 @@
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
-      <c r="U60" s="10" t="s">
+      <c r="U60" s="14" t="s">
         <v>5</v>
       </c>
       <c r="V60" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W60" s="2">
-        <f t="shared" ref="W60:Z60" si="8">AVERAGE(ABS(W10),ABS(W20),ABS(W30),ABS(W40),ABS(W50))</f>
+        <f t="shared" ref="W60:X60" si="8">AVERAGE(ABS(W10),ABS(W20),ABS(W30),ABS(W40),ABS(W50))</f>
         <v>0.23775255678971363</v>
       </c>
       <c r="X60" s="2">
         <f t="shared" si="8"/>
         <v>0.10386996855845942</v>
       </c>
+      <c r="Y60" s="11">
+        <v>5.4373999999999999E-2</v>
+      </c>
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="13:27" x14ac:dyDescent="0.25">
-      <c r="M61" s="10"/>
+      <c r="M61" s="14"/>
       <c r="N61" s="2" t="s">
         <v>33</v>
       </c>
@@ -4986,19 +5200,57 @@
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
-      <c r="U61" s="10"/>
+      <c r="U61" s="14"/>
       <c r="V61" s="2" t="s">
         <v>33</v>
       </c>
       <c r="W61" s="2">
-        <f t="shared" ref="W61:Z61" si="9">AVERAGE(ABS(W11),ABS(W21),ABS(W31),ABS(W41),ABS(W51))</f>
+        <f t="shared" ref="W61:X61" si="9">AVERAGE(ABS(W11),ABS(W21),ABS(W31),ABS(W41),ABS(W51))</f>
         <v>3.4631245452790463E-2</v>
       </c>
       <c r="X61" s="2">
         <f t="shared" si="9"/>
         <v>5.2445791483400096E-2</v>
       </c>
+      <c r="Y61" s="11">
+        <v>2.3941437399999996</v>
+      </c>
       <c r="AA61" s="2"/>
+    </row>
+    <row r="72" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y72" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y73" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y74" s="11">
+        <v>8.5971460000000013E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y75" s="11">
+        <v>5.9133000000000005E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y76" s="11">
+        <v>7.2414722999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y77" s="11">
+        <v>5.4373999999999999E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y78" s="11">
+        <v>2.3941437399999996</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -5008,6 +5260,8 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U17:U19"/>
+    <mergeCell ref="U20:U21"/>
     <mergeCell ref="U40:U41"/>
     <mergeCell ref="U47:U49"/>
     <mergeCell ref="U50:U51"/>
@@ -5016,8 +5270,6 @@
     <mergeCell ref="M37:M39"/>
     <mergeCell ref="M40:M41"/>
     <mergeCell ref="M47:M49"/>
-    <mergeCell ref="U17:U19"/>
-    <mergeCell ref="U20:U21"/>
     <mergeCell ref="U27:U29"/>
     <mergeCell ref="U30:U31"/>
     <mergeCell ref="U37:U39"/>
@@ -5042,4 +5294,1213 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BDE731-05DB-4D3F-A1F9-B4533E79758C}">
+  <dimension ref="B3:U54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>-2.8793809127398398E-3</v>
+      </c>
+      <c r="C6" s="10">
+        <v>3.8683136686680698E-2</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="10">
+        <v>3.9421889734320099E-2</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>6.0479026379282499E-2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.25159207939719302</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.1532713</v>
+      </c>
+      <c r="G7" s="10">
+        <v>-6.3075789744922506E-2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>6.8052350781593496E-2</v>
+      </c>
+      <c r="I7" s="10">
+        <v>7.7031500000000003E-2</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="10"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>6.1323183728548197E-2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.35425143874313397</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7.5840199999999997E-2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>-5.8444813385787601E-2</v>
+      </c>
+      <c r="H8" s="10">
+        <v>9.3970923868453002E-2</v>
+      </c>
+      <c r="I8" s="10">
+        <v>6.1461300000000003E-2</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="11"/>
+      <c r="U8" s="12"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
+        <v>5.7291661366381003E-2</v>
+      </c>
+      <c r="C9" s="10">
+        <v>-0.132699944940745</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.72831650000000003</v>
+      </c>
+      <c r="G9" s="10">
+        <v>5.4457146652880102E-2</v>
+      </c>
+      <c r="H9" s="10">
+        <v>-0.12667829139220699</v>
+      </c>
+      <c r="I9" s="10">
+        <v>7.5671590999999996</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9">
+        <v>-2.3126093995199E-2</v>
+      </c>
+      <c r="R9">
+        <v>0.231085100978006</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>5.9232215538854299E-2</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.65224561581443996</v>
+      </c>
+      <c r="D10" s="10">
+        <v>7.2989299999999993E-2</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-7.1247455342277194E-2</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.18826319540997299</v>
+      </c>
+      <c r="I10" s="10">
+        <v>5.12436E-2</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10">
+        <v>-3.13505852520643E-2</v>
+      </c>
+      <c r="R10">
+        <v>2.6280214976521599E-2</v>
+      </c>
+      <c r="S10">
+        <v>1.0381113</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>5.7115892953892397E-2</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.13810250461403301</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.59202849999999996</v>
+      </c>
+      <c r="G11" s="10">
+        <v>3.74904732350715E-2</v>
+      </c>
+      <c r="H11" s="10">
+        <v>7.6347757281711101E-2</v>
+      </c>
+      <c r="I11" s="10">
+        <v>2.591745</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11">
+        <v>-3.1663240102701599E-2</v>
+      </c>
+      <c r="R11">
+        <v>-4.4430223599136301E-2</v>
+      </c>
+      <c r="S11">
+        <v>0.34797109999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O12" s="14"/>
+      <c r="P12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12">
+        <v>-1.75299800637439E-2</v>
+      </c>
+      <c r="R12">
+        <v>2.64830628215171E-3</v>
+      </c>
+      <c r="S12">
+        <v>8.1442394</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13">
+        <v>3.1317090732169199E-2</v>
+      </c>
+      <c r="R13">
+        <v>-3.9080860436099797E-2</v>
+      </c>
+      <c r="S13">
+        <v>0.25826270000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O14" s="14"/>
+      <c r="P14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14">
+        <v>2.8245528371981701E-2</v>
+      </c>
+      <c r="R14">
+        <v>-4.39153254902825E-2</v>
+      </c>
+      <c r="S14">
+        <v>5.7578462999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>-2.9231597222833402E-3</v>
+      </c>
+      <c r="C15" s="10">
+        <v>9.8522551395139098E-3</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
+        <v>-1.61791266987041E-2</v>
+      </c>
+      <c r="H15" s="10">
+        <v>8.4494003124873495E-3</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="R15" s="11"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
+        <v>-0.258156948503794</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.105850436617139</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.10259459999999999</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.25838609245601801</v>
+      </c>
+      <c r="H16" s="10">
+        <v>2.4041685107463701E-2</v>
+      </c>
+      <c r="I16" s="10">
+        <v>7.4407699999999993E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>-0.26649192069316302</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.22813147473464801</v>
+      </c>
+      <c r="D17" s="10">
+        <v>6.8648500000000001E-2</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.25871731253959701</v>
+      </c>
+      <c r="H17" s="10">
+        <v>3.7722981033412602E-2</v>
+      </c>
+      <c r="I17" s="10">
+        <v>5.9511500000000002E-2</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>-0.24741993114291599</v>
+      </c>
+      <c r="C18" s="10">
+        <v>-1.7748203727189599E-3</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.71768920000000003</v>
+      </c>
+      <c r="G18" s="10">
+        <v>-0.13955392036956801</v>
+      </c>
+      <c r="H18" s="10">
+        <v>-3.5654096123447901E-2</v>
+      </c>
+      <c r="I18" s="10">
+        <v>7.4933551999999999</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <v>-0.25575553624060099</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.54933858943501501</v>
+      </c>
+      <c r="D19" s="10">
+        <v>6.0626399999999997E-2</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10">
+        <v>0.27338624055726002</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.37053138627841797</v>
+      </c>
+      <c r="I19" s="10">
+        <v>5.0475800000000001E-2</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q19">
+        <v>-2.0644148618710501E-2</v>
+      </c>
+      <c r="R19">
+        <v>5.3509661634034297E-2</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
+        <v>-0.25138248243977201</v>
+      </c>
+      <c r="C20" s="10">
+        <v>4.1077136596076799E-2</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.57745659999999999</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10">
+        <v>5.3480109544686801E-2</v>
+      </c>
+      <c r="H20" s="10">
+        <v>-2.0483877609899202E-2</v>
+      </c>
+      <c r="I20" s="10">
+        <v>2.4318610999999999</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20">
+        <v>3.2581273209340102E-2</v>
+      </c>
+      <c r="R20">
+        <v>1.57126985644658E-3</v>
+      </c>
+      <c r="S20">
+        <v>1.0324990000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21">
+        <v>3.2974704566981698E-2</v>
+      </c>
+      <c r="R21">
+        <v>1.06230516004455E-2</v>
+      </c>
+      <c r="S21">
+        <v>0.33124579999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22">
+        <v>-2.4514919073453399E-2</v>
+      </c>
+      <c r="R22">
+        <v>-1.1173425416172901E-2</v>
+      </c>
+      <c r="S22">
+        <v>8.1880412000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="10">
+        <v>3.1950702954274299E-3</v>
+      </c>
+      <c r="C23" s="10">
+        <v>9.2914714245845506E-3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10">
+        <v>-8.7530107045868197E-3</v>
+      </c>
+      <c r="H23" s="10">
+        <v>6.97533959348172E-3</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q23">
+        <v>2.9308734483464698E-2</v>
+      </c>
+      <c r="R23">
+        <v>2.4912245355478198E-2</v>
+      </c>
+      <c r="S23">
+        <v>0.2173834</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="10">
+        <v>0.32038734959588</v>
+      </c>
+      <c r="C24" s="10">
+        <v>6.7094878662945098E-2</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0.1012175</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
+        <v>0.346546172776314</v>
+      </c>
+      <c r="H24" s="10">
+        <v>6.3456413204267204E-2</v>
+      </c>
+      <c r="I24" s="10">
+        <v>7.5579400000000005E-2</v>
+      </c>
+      <c r="O24" s="14"/>
+      <c r="P24" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24">
+        <v>-1.24241742405469E-2</v>
+      </c>
+      <c r="R24">
+        <v>2.6664877632007799E-3</v>
+      </c>
+      <c r="S24">
+        <v>5.7910086999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="10">
+        <v>0.33406714898026102</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.20001183088282601</v>
+      </c>
+      <c r="D25" s="10">
+        <v>6.8552500000000002E-2</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.34662165246011201</v>
+      </c>
+      <c r="H25" s="10">
+        <v>7.3068304599831199E-2</v>
+      </c>
+      <c r="I25" s="10">
+        <v>6.03939E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="10">
+        <v>-0.31213269381592201</v>
+      </c>
+      <c r="C26" s="10">
+        <v>6.2049362798483297E-2</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.71639640000000004</v>
+      </c>
+      <c r="G26" s="10">
+        <v>-0.17445758212745799</v>
+      </c>
+      <c r="H26" s="10">
+        <v>-4.3928122940248698E-2</v>
+      </c>
+      <c r="I26" s="10">
+        <v>7.5173126999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="10">
+        <v>0.31100421319931698</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0.53302208853138</v>
+      </c>
+      <c r="D27" s="10">
+        <v>6.4356499999999997E-2</v>
+      </c>
+      <c r="G27" s="10">
+        <v>-0.35129919094655299</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0.362901872099818</v>
+      </c>
+      <c r="I27" s="10">
+        <v>5.09919E-2</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="10">
+        <v>-0.31665494175985898</v>
+      </c>
+      <c r="C28" s="10">
+        <v>-2.08578304095237E-2</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.57737870000000002</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="10">
+        <v>7.7322423331664897E-4</v>
+      </c>
+      <c r="I28" s="10">
+        <v>2.4416547999999998</v>
+      </c>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>46</v>
+      </c>
+      <c r="R29">
+        <v>5.4010932604653103E-2</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="O30" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q30">
+        <v>3.2884897285117301E-2</v>
+      </c>
+      <c r="R30">
+        <v>2.0844957559215001E-2</v>
+      </c>
+      <c r="S30">
+        <v>1.014869</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="10">
+        <v>-4.7494459413725196E-3</v>
+      </c>
+      <c r="C31" s="10">
+        <v>8.4064353556593495E-3</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10">
+        <v>-1.30769365249208E-2</v>
+      </c>
+      <c r="H31" s="10">
+        <v>2.52443522105707E-3</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0</v>
+      </c>
+      <c r="O31" s="14"/>
+      <c r="P31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q31">
+        <v>3.5825343323010302E-2</v>
+      </c>
+      <c r="R31">
+        <v>1.40286618171639E-3</v>
+      </c>
+      <c r="S31">
+        <v>0.32259870000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="10">
+        <v>-0.14203520776123599</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0.127763060397626</v>
+      </c>
+      <c r="D32" s="10">
+        <v>9.8708900000000002E-2</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10">
+        <v>-0.119889215233867</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0.58918096309422896</v>
+      </c>
+      <c r="I32" s="10">
+        <v>7.6005199999999995E-2</v>
+      </c>
+      <c r="O32" s="14"/>
+      <c r="P32" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32">
+        <v>-2.63552810156313E-2</v>
+      </c>
+      <c r="R32">
+        <v>-1.0911749246723499E-2</v>
+      </c>
+      <c r="S32">
+        <v>8.2370657999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="10">
+        <v>-0.143135157194693</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0.19530948322564801</v>
+      </c>
+      <c r="D33" s="10">
+        <v>7.0705299999999999E-2</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10">
+        <v>-0.115541143115856</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0.612347799491051</v>
+      </c>
+      <c r="I33" s="10">
+        <v>6.0996700000000001E-2</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P33" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q33">
+        <v>-3.7563711077636501E-2</v>
+      </c>
+      <c r="R33">
+        <v>1.20343657774311E-2</v>
+      </c>
+      <c r="S33">
+        <v>0.2049822</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="10">
+        <v>-0.116651803756077</v>
+      </c>
+      <c r="C34" s="10">
+        <v>-5.0446080950753203E-2</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0.71557329999999997</v>
+      </c>
+      <c r="G34" s="10">
+        <v>5.62888969065597E-2</v>
+      </c>
+      <c r="H34" s="10">
+        <v>2.3462040446012799E-3</v>
+      </c>
+      <c r="I34" s="10">
+        <v>7.5143243000000002</v>
+      </c>
+      <c r="O34" s="14"/>
+      <c r="P34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>46</v>
+      </c>
+      <c r="R34">
+        <v>1.27286933791768E-2</v>
+      </c>
+      <c r="S34">
+        <v>5.9709310000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="10">
+        <v>-0.13268105107336101</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0.44593000426573798</v>
+      </c>
+      <c r="D35" s="10">
+        <v>6.1481599999999997E-2</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0.127587110355497</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0.68595205254664204</v>
+      </c>
+      <c r="I35" s="10">
+        <v>5.03445E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B36" s="10">
+        <v>-0.119056885276373</v>
+      </c>
+      <c r="C36" s="10">
+        <v>-3.6020870277646097E-2</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0.58403450000000001</v>
+      </c>
+      <c r="G36" s="10">
+        <v>2.4785035356638299E-2</v>
+      </c>
+      <c r="H36" s="10">
+        <v>-1.47147614911527E-4</v>
+      </c>
+      <c r="I36" s="10">
+        <v>2.4350664000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O37" s="11"/>
+      <c r="P37" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R38" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S38" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B39" s="10">
+        <v>4.1242263285340801E-3</v>
+      </c>
+      <c r="C39" s="10">
+        <v>9.1592986991269505E-3</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10">
+        <v>9.6551651831113493E-3</v>
+      </c>
+      <c r="H39" s="10">
+        <v>8.0087794877463196E-3</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0</v>
+      </c>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q39">
+        <v>-2.0168461264879901E-2</v>
+      </c>
+      <c r="R39">
+        <v>4.2396762954001903E-2</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B40" s="10">
+        <v>0.32783811028699</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0.12799740749540001</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0.1012955</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0.36293182023454401</v>
+      </c>
+      <c r="H40" s="10">
+        <v>0.119705061597014</v>
+      </c>
+      <c r="I40" s="10">
+        <v>7.4240299999999995E-2</v>
+      </c>
+      <c r="O40" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q40">
+        <v>-1.6063427324618001E-2</v>
+      </c>
+      <c r="R40">
+        <v>8.8058569042983592E-3</v>
+      </c>
+      <c r="S40">
+        <v>1.0432855000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B41" s="10">
+        <v>0.32248397785518501</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0.24604854097746201</v>
+      </c>
+      <c r="D41" s="10">
+        <v>6.8163199999999993E-2</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0.36992104672084303</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0.129209991712916</v>
+      </c>
+      <c r="I41" s="10">
+        <v>5.9176199999999998E-2</v>
+      </c>
+      <c r="O41" s="14"/>
+      <c r="P41" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q41">
+        <v>-1.4886551401657599E-2</v>
+      </c>
+      <c r="R41">
+        <v>6.1912660867031698E-3</v>
+      </c>
+      <c r="S41">
+        <v>0.32760400000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B42" s="10">
+        <v>0.36759840173983099</v>
+      </c>
+      <c r="C42" s="10">
+        <v>-9.1577658240258902E-2</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.7251533</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0.20536007892006899</v>
+      </c>
+      <c r="H42" s="10">
+        <v>1.36548198314422E-2</v>
+      </c>
+      <c r="I42" s="10">
+        <v>7.5283243000000004</v>
+      </c>
+      <c r="O42" s="14"/>
+      <c r="P42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q42">
+        <v>1.09551509155756E-2</v>
+      </c>
+      <c r="R42">
+        <v>2.28873493444016E-3</v>
+      </c>
+      <c r="S42">
+        <v>8.1518177999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B43" s="10">
+        <v>0.34470824386962501</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0.49377157854361098</v>
+      </c>
+      <c r="D43" s="10">
+        <v>6.0599500000000001E-2</v>
+      </c>
+      <c r="G43" s="10">
+        <v>-0.36524278674698102</v>
+      </c>
+      <c r="H43" s="10">
+        <v>0.42319604951492901</v>
+      </c>
+      <c r="I43" s="10">
+        <v>5.0078499999999998E-2</v>
+      </c>
+      <c r="O43" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q43">
+        <v>-1.44212796250228E-2</v>
+      </c>
+      <c r="R43">
+        <v>-1.11584211195132E-2</v>
+      </c>
+      <c r="S43">
+        <v>0.2163445</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B44" s="10">
+        <v>0.36667219765792303</v>
+      </c>
+      <c r="C44" s="10">
+        <v>-0.23276710783753099</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.57683689999999999</v>
+      </c>
+      <c r="G44" s="10">
+        <v>5.74006091275557E-2</v>
+      </c>
+      <c r="H44" s="10">
+        <v>9.7010898010628493E-3</v>
+      </c>
+      <c r="I44" s="10">
+        <v>2.4213705999999999</v>
+      </c>
+      <c r="O44" s="14"/>
+      <c r="P44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44">
+        <v>-1.37094355455647E-2</v>
+      </c>
+      <c r="R44">
+        <v>-3.6135346949242699E-3</v>
+      </c>
+      <c r="S44">
+        <v>5.8122530000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O47" s="11"/>
+      <c r="P47" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R48" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S48" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O49" s="11"/>
+      <c r="P49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q49">
+        <v>-2.1411951880423299E-2</v>
+      </c>
+      <c r="R49">
+        <v>4.6446502986740801E-2</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O50" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P50" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q50">
+        <v>3.2790531286727403E-2</v>
+      </c>
+      <c r="R50">
+        <v>1.8131130459553599E-2</v>
+      </c>
+      <c r="S50">
+        <v>1.0325983000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O51" s="14"/>
+      <c r="P51" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q51">
+        <v>3.2548870805133301E-2</v>
+      </c>
+      <c r="R51">
+        <v>1.46864870583341E-2</v>
+      </c>
+      <c r="S51">
+        <v>0.35760999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O52" s="14"/>
+      <c r="P52" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q52">
+        <v>2.7095071818930599E-2</v>
+      </c>
+      <c r="R52">
+        <v>4.2065850655324801E-3</v>
+      </c>
+      <c r="S52">
+        <v>8.1015450999999992</v>
+      </c>
+    </row>
+    <row r="53" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O53" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P53" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q53">
+        <v>-3.4038180261612101E-2</v>
+      </c>
+      <c r="R53">
+        <v>7.7162714589709596E-3</v>
+      </c>
+      <c r="S53">
+        <v>0.21489269999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O54" s="14"/>
+      <c r="P54" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q54">
+        <v>2.2848201838338002E-2</v>
+      </c>
+      <c r="R54">
+        <v>-4.80215838039228E-4</v>
+      </c>
+      <c r="S54">
+        <v>5.7573980000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O20:O22"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="O33:O34"/>
+    <mergeCell ref="O40:O42"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="O50:O52"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>